<commit_message>
Radar plots and code, text and minor updates
</commit_message>
<xml_diff>
--- a/classification_report.xlsx
+++ b/classification_report.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Res1" sheetId="1" r:id="rId1"/>
     <sheet name="Res2" sheetId="2" r:id="rId2"/>
     <sheet name="19012017" sheetId="3" r:id="rId3"/>
     <sheet name="20012017" sheetId="4" r:id="rId4"/>
+    <sheet name="07022017" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -170,8 +171,44 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Shadrina, Alina</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Shadrina, Alina:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3124" uniqueCount="295">
   <si>
     <t>резиночки желтые</t>
   </si>
@@ -1080,12 +1117,1217 @@
     <t>benzol
 etilazetat</t>
   </si>
+  <si>
+    <t>benzol;dioktilftalat;etilazetat</t>
+  </si>
+  <si>
+    <t>benzol;dioktilftalat</t>
+  </si>
+  <si>
+    <t>azetal_degid;benzin;dioktilftalat</t>
+  </si>
+  <si>
+    <t>benzol;etilazetat</t>
+  </si>
+  <si>
+    <t>etilazetat;plastizol_</t>
+  </si>
+  <si>
+    <t>azetal_degid;dioktilftalat</t>
+  </si>
+  <si>
+    <t>benzin;fenol;toluol</t>
+  </si>
+  <si>
+    <t>propanol</t>
+  </si>
+  <si>
+    <t>azetal_degid;dioktilftalat;propanol</t>
+  </si>
+  <si>
+    <t>azetal_degid;azeton;plastizol_</t>
+  </si>
+  <si>
+    <t>azetal_degid;benzol;etilazetat</t>
+  </si>
+  <si>
+    <t>azetal_degid;azeton;dioktilftalat;plastizol_</t>
+  </si>
+  <si>
+    <t>dioktilftalat;etilazetat</t>
+  </si>
+  <si>
+    <t>azeton;benzin;dioktilftalat</t>
+  </si>
+  <si>
+    <t>dioktilftalat;izobutanol</t>
+  </si>
+  <si>
+    <t>benzin;izopropanol;plastizol_;stirol;toluol</t>
+  </si>
+  <si>
+    <t>azetal_degid;dioktilftalat;propanol;toluol</t>
+  </si>
+  <si>
+    <t>azetal_degid;azeton;butilazetat;dioktilftalat;fenol</t>
+  </si>
+  <si>
+    <t>azeton;etilazetat</t>
+  </si>
+  <si>
+    <t>azetal_degid;benzol</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ацетон</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>azeton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;etilazetat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Диоктилфталат
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ацетон</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Толуол
+Бензол
+Ацетальдегид
+Ацетон</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Толуол
+Бензол
+Ацетальдегид
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ацетон</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ДОФ
+с этилацетатом
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ацетон</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>azetal_degid;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dioktilftalat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ацетон</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>azeton;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>etilazetat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Этилацетат
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ацетон
+Изобутиловый спирт</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Этилацетат
+Ацетальдегид
+Ацетон
+Толуол
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Бензол</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Фенол</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>benzol;dioktilftalat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;plastizol_</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>azetal_degid;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dioktilftalat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;propanol</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Керосин
+Диоктилфталат
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ацетальдегид</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Бензол
+Изопропиловый спирт</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>azetal_degid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;benzol;etilazetat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Гексан
+ДОФ с бензолом
+ДОФ с ацетальдегидом
+Толуол
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Бензол</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Стирол
+Ацетальдегид</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Гексан</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Диоктилфталат
+Бутилацетат
+Бензол</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Гексан
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Бутилацетат
+Бензол</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>azetal_degid;etilazetat;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>geksan</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Этилацетат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ацетальдегид
+Бутилацетат
+Изопропанол
+Бензол
+Толуол
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>azeton;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>etilazeta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t;plastizol_</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Этилацетат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Изобутиловый спирт</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ацетон
+Ацетальдегид
+Этилацетат
+Бутилацетат</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Этилацетат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ацетальдегид</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dioktilftalat;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>etilazetat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;fenol</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Этилацетат
+Бензол
+Толуол
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Бензол</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ацетальдегид</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Толуол
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>azetal_degid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;azeton;benzin</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;benzo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l;butilazetat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>benzo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l;stirol</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Фенол
+Ацетон
+Ацетальдегид
+Толуол
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Бензол</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Диоктилфталат</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Фенол
+Толуол
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Бензол</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ацетон</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Стирол
+Ацетальдегид
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Этилацетат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Бутилацетат
+Бензол
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Изобутанол
+Ацетальдегид
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Этилацетат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Бутилацетат
+Изопропанол
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>azeton;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>etilazetat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Толуол
+Ацетальдегид
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Диоктилфталат</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Изопропанол</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>azeton;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dioktilftalat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>izopropanol</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;stirol</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">бутанол 
+изобутанол
+пропанол
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>изопропанол</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1159,8 +2401,32 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1173,8 +2439,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1197,11 +2475,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1294,6 +2598,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8754,8 +10082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H76" sqref="A1:H76"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9048,7 +10376,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -9338,7 +10666,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -9396,7 +10724,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -9512,7 +10840,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>25</v>
       </c>
@@ -9686,7 +11014,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>31</v>
       </c>
@@ -10063,7 +11391,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
         <v>44</v>
       </c>
@@ -10121,7 +11449,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A47" s="14">
         <v>46</v>
       </c>
@@ -10353,7 +11681,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A55" s="14">
         <v>54</v>
       </c>
@@ -10643,7 +11971,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
         <v>64</v>
       </c>
@@ -11002,4 +12330,2031 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" customWidth="1"/>
+    <col min="12" max="12" width="80.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="32"/>
+    </row>
+    <row r="3" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="L3" s="32"/>
+    </row>
+    <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="L4" s="32"/>
+    </row>
+    <row r="5" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="L5" s="32"/>
+    </row>
+    <row r="6" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="L6" s="32"/>
+    </row>
+    <row r="7" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="L7" s="32"/>
+    </row>
+    <row r="8" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="L8" s="32"/>
+    </row>
+    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="81.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="84.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>14</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>15</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>16</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>20</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>21</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>22</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>23</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>26</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>27</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>28</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>29</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>30</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>31</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>32</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="G33" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>33</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>34</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>35</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>36</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="14">
+        <v>37</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
+        <v>38</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>39</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H40" s="21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
+        <v>40</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>41</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
+        <v>42</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
+        <v>43</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H44" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>44</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H45" s="20" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
+        <v>45</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>46</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H47" s="20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="14">
+        <v>47</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="H48" s="20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
+        <v>48</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="H49" s="21" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
+        <v>49</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="H50" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+      <c r="A51" s="14">
+        <v>50</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F51" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G51" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="H51" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+      <c r="A52" s="14">
+        <v>51</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G52" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="H52" s="21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="14">
+        <v>52</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G53" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H53" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="14">
+        <v>53</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H54" s="21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="14">
+        <v>54</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G55" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H55" s="21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="116.25" x14ac:dyDescent="0.25">
+      <c r="A56" s="14">
+        <v>55</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G56" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="14">
+        <v>56</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H57" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="14">
+        <v>57</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G58" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H58" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="14">
+        <v>58</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G59" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="14">
+        <v>59</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G60" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="14">
+        <v>60</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H61" s="21" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="14">
+        <v>61</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H62" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="14">
+        <v>62</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H63" s="20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="81.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="14">
+        <v>63</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C64" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F64" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G64" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="14">
+        <v>64</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C65" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G65" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="H65" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A66" s="14">
+        <v>65</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D66" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G66" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="H66" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="N66">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
+        <v>66</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="G67" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="H67" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A68" s="14">
+        <v>67</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="D68" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G68" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="H68" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="97.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="14">
+        <v>68</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C69" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="H69" s="20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="66" x14ac:dyDescent="0.25">
+      <c r="A70" s="14">
+        <v>69</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G70" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="H70" s="20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="14">
+        <v>70</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="D71" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G71" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="H71" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="14">
+        <v>71</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C72" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D72" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F72" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="G72" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="H72" s="20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A73" s="14">
+        <v>72</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D73" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G73" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="H73" s="20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="14">
+        <v>73</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C74" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="D74" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="E74" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F74" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G74" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="H74" s="20" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="66" x14ac:dyDescent="0.25">
+      <c r="A75" s="14">
+        <v>74</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C75" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F75" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G75" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="H75" s="20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A76" s="14">
+        <v>75</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G76" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="H76" s="21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L1:L8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>